<commit_message>
se agrega config.ini para la configuración de la automatización
</commit_message>
<xml_diff>
--- a/resultado_final.xlsx
+++ b/resultado_final.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basti\OneDrive\Escritorio\proyecto CENCOSUD\Automatizacion Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36127410-6219-4AC7-BDDA-55EECAF41CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C5F1AA-44EB-48C9-BFC1-17430295210A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="42">
   <si>
     <t>Mes</t>
   </si>
@@ -58,97 +58,94 @@
     <t>Juan Pérez</t>
   </si>
   <si>
+    <t>Ana López</t>
+  </si>
+  <si>
+    <t>Carlos Ruiz</t>
+  </si>
+  <si>
+    <t>Marta Díaz</t>
+  </si>
+  <si>
+    <t>Luis Torres</t>
+  </si>
+  <si>
+    <t>Carla Gómez</t>
+  </si>
+  <si>
+    <t>Jorge Ramírez</t>
+  </si>
+  <si>
+    <t>Sofia Martínez</t>
+  </si>
+  <si>
+    <t>Pedro Cabrera</t>
+  </si>
+  <si>
+    <t>Laura Núñez</t>
+  </si>
+  <si>
+    <t>Tomás Vázquez</t>
+  </si>
+  <si>
+    <t>Paula Fernández</t>
+  </si>
+  <si>
+    <t>Antonio Soto</t>
+  </si>
+  <si>
+    <t>Isabel Rivas</t>
+  </si>
+  <si>
+    <t>Daniel Ortiz</t>
+  </si>
+  <si>
+    <t>Mariana Mendoza</t>
+  </si>
+  <si>
+    <t>Javier Cruz</t>
+  </si>
+  <si>
+    <t>Nuria Escribano</t>
+  </si>
+  <si>
+    <t>Francisco León</t>
+  </si>
+  <si>
+    <t>Carmen Molina</t>
+  </si>
+  <si>
     <t>Sales</t>
   </si>
   <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
     <t>BB</t>
   </si>
   <si>
-    <t>Ana López</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
     <t>AB</t>
   </si>
   <si>
-    <t>Carlos Ruiz</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>Marta Díaz</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
     <t>AA</t>
   </si>
   <si>
-    <t>Luis Torres</t>
-  </si>
-  <si>
-    <t>Carla Gómez</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>Jorge Ramírez</t>
-  </si>
-  <si>
-    <t>Sofia Martínez</t>
-  </si>
-  <si>
-    <t>Pedro Cabrera</t>
-  </si>
-  <si>
     <t>BA</t>
   </si>
   <si>
-    <t>Laura Núñez</t>
-  </si>
-  <si>
     <t>CB</t>
   </si>
   <si>
-    <t>Tomás Vázquez</t>
-  </si>
-  <si>
-    <t>Paula Fernández</t>
-  </si>
-  <si>
     <t>AC</t>
-  </si>
-  <si>
-    <t>Antonio Soto</t>
-  </si>
-  <si>
-    <t>Isabel Rivas</t>
-  </si>
-  <si>
-    <t>Daniel Ortiz</t>
-  </si>
-  <si>
-    <t>Mariana Mendoza</t>
-  </si>
-  <si>
-    <t>Javier Cruz</t>
-  </si>
-  <si>
-    <t>Nuria Escribano</t>
-  </si>
-  <si>
-    <t>Francisco León</t>
-  </si>
-  <si>
-    <t>Carmen Molina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allison </t>
   </si>
 </sst>
 </file>
@@ -156,7 +153,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -169,7 +166,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -231,9 +231,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -271,7 +271,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -305,6 +305,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -339,9 +340,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -515,22 +517,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K62" sqref="K62"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -580,10 +579,10 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F2">
         <v>750000</v>
@@ -612,13 +611,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F3">
         <v>900000</v>
@@ -647,13 +646,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F4">
         <v>825000</v>
@@ -682,13 +681,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="F5">
         <v>1050000</v>
@@ -717,13 +716,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F6">
         <v>780000</v>
@@ -752,13 +751,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F7">
         <v>975000</v>
@@ -787,13 +786,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F8">
         <v>870000</v>
@@ -822,13 +821,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F9">
         <v>1080000</v>
@@ -857,13 +856,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F10">
         <v>795000</v>
@@ -892,13 +891,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F11">
         <v>945000</v>
@@ -927,13 +926,13 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F12">
         <v>990000</v>
@@ -962,13 +961,13 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F13">
         <v>825000</v>
@@ -997,13 +996,13 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
         <v>34</v>
       </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F14">
         <v>1125000</v>
@@ -1032,13 +1031,13 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F15">
         <v>855000</v>
@@ -1067,13 +1066,13 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F16">
         <v>960000</v>
@@ -1102,13 +1101,13 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F17">
         <v>1020000</v>
@@ -1137,13 +1136,13 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F18">
         <v>765000</v>
@@ -1172,13 +1171,13 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F19">
         <v>1110000</v>
@@ -1207,13 +1206,13 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F20">
         <v>840000</v>
@@ -1242,13 +1241,13 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F21">
         <v>930000</v>
@@ -1280,10 +1279,10 @@
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F22">
         <v>772500</v>
@@ -1312,13 +1311,13 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F23">
         <v>927000</v>
@@ -1347,13 +1346,13 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F24">
         <v>849750</v>
@@ -1382,13 +1381,13 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="F25">
         <v>1081500</v>
@@ -1417,13 +1416,13 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F26">
         <v>803400</v>
@@ -1452,13 +1451,13 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F27">
         <v>1004250</v>
@@ -1487,13 +1486,13 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F28">
         <v>896100</v>
@@ -1522,13 +1521,13 @@
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F29">
         <v>1112400</v>
@@ -1557,13 +1556,13 @@
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E30" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F30">
         <v>818850</v>
@@ -1592,13 +1591,13 @@
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E31" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F31">
         <v>973350</v>
@@ -1627,13 +1626,13 @@
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D32" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F32">
         <v>1019700</v>
@@ -1662,13 +1661,13 @@
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F33">
         <v>849750</v>
@@ -1697,13 +1696,13 @@
         <v>13</v>
       </c>
       <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" t="s">
         <v>34</v>
       </c>
-      <c r="D34" t="s">
-        <v>20</v>
-      </c>
       <c r="E34" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F34">
         <v>1158750</v>
@@ -1732,13 +1731,13 @@
         <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F35">
         <v>880650</v>
@@ -1767,13 +1766,13 @@
         <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E36" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F36">
         <v>988800</v>
@@ -1802,13 +1801,13 @@
         <v>16</v>
       </c>
       <c r="C37" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F37">
         <v>1050600</v>
@@ -1837,13 +1836,13 @@
         <v>17</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E38" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F38">
         <v>787950</v>
@@ -1872,13 +1871,13 @@
         <v>18</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D39" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E39" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F39">
         <v>1143300</v>
@@ -1907,13 +1906,13 @@
         <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D40" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E40" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F40">
         <v>865200</v>
@@ -1942,13 +1941,13 @@
         <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D41" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E41" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F41">
         <v>957900</v>
@@ -1980,10 +1979,10 @@
         <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E42" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F42">
         <v>772500</v>
@@ -2012,13 +2011,13 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D43" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E43" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F43">
         <v>927000</v>
@@ -2047,13 +2046,13 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E44" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F44">
         <v>849750</v>
@@ -2082,13 +2081,13 @@
         <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D45" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E45" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="F45">
         <v>1081500</v>
@@ -2117,13 +2116,13 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E46" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F46">
         <v>883740</v>
@@ -2152,13 +2151,13 @@
         <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D47" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E47" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="G47">
         <v>0.14000000000000001</v>
@@ -2178,13 +2177,13 @@
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D48" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E48" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F48">
         <v>896100</v>
@@ -2213,13 +2212,13 @@
         <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F49">
         <v>1279260</v>
@@ -2248,13 +2247,13 @@
         <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D50" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E50" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F50">
         <v>818850</v>
@@ -2283,13 +2282,13 @@
         <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D51" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E51" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F51">
         <v>973350</v>
@@ -2318,13 +2317,13 @@
         <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D52" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E52" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F52">
         <v>1121670</v>
@@ -2353,13 +2352,13 @@
         <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D53" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E53" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F53">
         <v>849750</v>
@@ -2388,13 +2387,13 @@
         <v>13</v>
       </c>
       <c r="C54" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" t="s">
         <v>34</v>
       </c>
-      <c r="D54" t="s">
-        <v>20</v>
-      </c>
       <c r="E54" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F54">
         <v>1158750</v>
@@ -2423,13 +2422,13 @@
         <v>14</v>
       </c>
       <c r="C55" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D55" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E55" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="G55">
         <v>0.11</v>
@@ -2449,13 +2448,13 @@
         <v>15</v>
       </c>
       <c r="C56" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D56" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E56" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F56">
         <v>988800</v>
@@ -2484,13 +2483,13 @@
         <v>16</v>
       </c>
       <c r="C57" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D57" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E57" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F57">
         <v>1050600</v>
@@ -2519,13 +2518,13 @@
         <v>17</v>
       </c>
       <c r="C58" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D58" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E58" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F58">
         <v>866745.00000000012</v>
@@ -2554,13 +2553,13 @@
         <v>18</v>
       </c>
       <c r="C59" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D59" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E59" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F59">
         <v>1143300</v>
@@ -2589,13 +2588,13 @@
         <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D60" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E60" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F60">
         <v>994979.99999999988</v>
@@ -2624,13 +2623,13 @@
         <v>20</v>
       </c>
       <c r="C61" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D61" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E61" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F61">
         <v>957900</v>
@@ -2651,42 +2650,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A62" s="2">
-        <v>45383</v>
-      </c>
-      <c r="B62">
-        <v>21</v>
-      </c>
-      <c r="C62" t="s">
-        <v>42</v>
-      </c>
-      <c r="D62" t="s">
-        <v>15</v>
-      </c>
-      <c r="E62" t="s">
-        <v>13</v>
-      </c>
-      <c r="F62">
-        <v>957900</v>
-      </c>
-      <c r="G62">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="H62">
-        <v>143685</v>
-      </c>
-      <c r="I62">
-        <v>1101585</v>
-      </c>
-      <c r="J62" s="2">
-        <v>40876</v>
-      </c>
-      <c r="K62">
-        <v>149</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>